<commit_message>
Thu PM Update 3p
</commit_message>
<xml_diff>
--- a/EmployeeSQL/Rodgers_ERD.xlsx
+++ b/EmployeeSQL/Rodgers_ERD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\Documents\sql-challenge\EmployeeSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF8BA7-09DD-4E06-9543-8A648F070460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EB7D1D-28A0-46B7-8CB7-4553C2A05345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1178E2C9-5C18-4B10-8129-0E9588271537}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>dept_no</t>
   </si>
@@ -151,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -314,9 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -326,6 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,82 +553,139 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312333</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Freeform: Shape 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42E748E-3E5E-41D4-860F-9DDE25461F68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362613" y="2682240"/>
+          <a:ext cx="716367" cy="868680"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 678267 w 716367"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 868680"/>
+            <a:gd name="connsiteX1" fmla="*/ 87 w 716367"/>
+            <a:gd name="connsiteY1" fmla="*/ 571500 h 868680"/>
+            <a:gd name="connsiteX2" fmla="*/ 716367 w 716367"/>
+            <a:gd name="connsiteY2" fmla="*/ 868680 h 868680"/>
+            <a:gd name="connsiteX3" fmla="*/ 716367 w 716367"/>
+            <a:gd name="connsiteY3" fmla="*/ 868680 h 868680"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="716367" h="868680">
+              <a:moveTo>
+                <a:pt x="678267" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="336002" y="213360"/>
+                <a:pt x="-6263" y="426720"/>
+                <a:pt x="87" y="571500"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6437" y="716280"/>
+                <a:pt x="716367" y="868680"/>
+                <a:pt x="716367" y="868680"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="716367" y="868680"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Straight Connector 12">
+        <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{094005B5-BD3B-49E0-A0DD-DC66AAF98E7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{535B00B4-B9BE-4974-8211-F78871ED57BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3322320" y="3390900"/>
-          <a:ext cx="4038600" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3988537-7705-49A5-886A-EDD4738D3FFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3048000" y="2682240"/>
-          <a:ext cx="3977640" cy="1082040"/>
+        <a:xfrm>
+          <a:off x="3078480" y="3764280"/>
+          <a:ext cx="3916680" cy="7620"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -947,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F0DF4-23BC-4349-BF66-E85E31894105}">
   <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,19 +1036,19 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="G4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="G4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -994,7 +1057,7 @@
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -1023,13 +1086,13 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="18"/>
       <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1048,11 +1111,11 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="G9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1096,27 +1159,27 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="G12" s="7" t="s">
+      <c r="D12" s="18"/>
+      <c r="G12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="14"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="L14" s="1" t="s">
@@ -1126,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -1137,36 +1200,36 @@
         <v>3</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="17" t="s">
+      <c r="M16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="18"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="L19" s="12" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="L19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="14"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
@@ -1175,9 +1238,7 @@
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D20" s="6"/>
       <c r="L20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>1</v>
@@ -1207,18 +1268,18 @@
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="L22" s="7" t="s">
+      <c r="D22" s="18"/>
+      <c r="L22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="8"/>
-      <c r="N22" s="9"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>